<commit_message>
fix bugs and add generate for up and down week
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>№ п/п</t>
   </si>
@@ -27,6 +27,9 @@
     <t>Дата</t>
   </si>
   <si>
+    <t>День недели</t>
+  </si>
+  <si>
     <t>Факультет, курс, группа</t>
   </si>
   <si>
@@ -36,22 +39,103 @@
     <t>Часы</t>
   </si>
   <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Основы разработки информационных систем</t>
+    <t>179</t>
+  </si>
+  <si>
+    <t>Базы данных</t>
   </si>
   <si>
     <t>February</t>
   </si>
   <si>
-    <t>ПИ-Б23-1-1 /ИИСГТ/Бак./ОФО</t>
+    <t>Вторник</t>
+  </si>
+  <si>
+    <t>БИ-Б22-1 /ИИСГТ/Бак./ОФО</t>
+  </si>
+  <si>
+    <t>Экзамен</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>Проектирование информационных систем</t>
+  </si>
+  <si>
+    <t>Понедельник</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>253</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>Профессиональная коммуникация системного аналитика</t>
+  </si>
+  <si>
+    <t>ПИ-Б23-1-1, ПИ-Б23-1-2 /ИИСГТ/Бак./ОФО</t>
   </si>
   <si>
     <t>Лекционные</t>
   </si>
   <si>
-    <t>11</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -418,7 +502,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -432,6 +516,7 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.5"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.5"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -453,25 +538,652 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generate with date and filter by weekType
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>№ п/п</t>
   </si>
@@ -30,6 +30,9 @@
     <t>День недели</t>
   </si>
   <si>
+    <t>Тип недели</t>
+  </si>
+  <si>
     <t>Факультет, курс, группа</t>
   </si>
   <si>
@@ -37,6 +40,90 @@
   </si>
   <si>
     <t>Часы</t>
+  </si>
+  <si>
+    <t>253</t>
+  </si>
+  <si>
+    <t>Проектирование информационных систем</t>
+  </si>
+  <si>
+    <t>2024-02-05 00:00:00 +0000 UTC</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Нижняя</t>
+  </si>
+  <si>
+    <t>БИ-Б22-1 /ИИСГТ/Бак./ОФО</t>
+  </si>
+  <si>
+    <t>Экзамен</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>Базы данных</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>2024-02-06 00:00:00 +0000 UTC</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2024-02-12 00:00:00 +0000 UTC</t>
+  </si>
+  <si>
+    <t>Верхняя</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>2024-02-13 00:00:00 +0000 UTC</t>
+  </si>
+  <si>
+    <t>2024-02-19 00:00:00 +0000 UTC</t>
+  </si>
+  <si>
+    <t>2024-02-20 00:00:00 +0000 UTC</t>
+  </si>
+  <si>
+    <t>2024-02-26 00:00:00 +0000 UTC</t>
+  </si>
+  <si>
+    <t>2024-02-27 00:00:00 +0000 UTC</t>
   </si>
 </sst>
 </file>
@@ -403,7 +490,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -418,6 +505,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.5"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.5"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -441,6 +529,1257 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>